<commit_message>
Final changes in time series code
</commit_message>
<xml_diff>
--- a/LR results.xlsx
+++ b/LR results.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CIT\Project\Air-Quality-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D4953E1-3FE9-4980-A3D6-193A42C79D56}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F211BD64-3DCA-43A2-BA0C-470604A53312}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{CE06976A-A07C-44A5-B586-F8D095DCA576}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Linear Regression" sheetId="1" r:id="rId1"/>
+    <sheet name="Time series" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="19">
   <si>
     <t>Stations</t>
   </si>
@@ -60,9 +61,6 @@
     <t>Waterford</t>
   </si>
   <si>
-    <t>Normal</t>
-  </si>
-  <si>
     <t>Standard Scalar</t>
   </si>
   <si>
@@ -70,13 +68,37 @@
   </si>
   <si>
     <t>Hyper Parameter Tuning</t>
+  </si>
+  <si>
+    <t>Original values</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>ETS</t>
+  </si>
+  <si>
+    <t>ARIMA</t>
+  </si>
+  <si>
+    <t>tslm</t>
+  </si>
+  <si>
+    <t>hourly</t>
+  </si>
+  <si>
+    <t>Daily</t>
+  </si>
+  <si>
+    <t>Monthly</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,22 +107,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -109,20 +124,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFF2F2F2"/>
       </patternFill>
     </fill>
   </fills>
@@ -135,44 +137,41 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.39997558519241921"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Heading 3" xfId="1" builtinId="18"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Output" xfId="1" builtinId="21"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -487,99 +486,103 @@
   <dimension ref="A1:Q13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="11.81640625" customWidth="1"/>
-    <col min="4" max="4" width="11.54296875" customWidth="1"/>
-    <col min="5" max="5" width="10" customWidth="1"/>
-    <col min="9" max="9" width="9.6328125" customWidth="1"/>
-    <col min="13" max="13" width="9.36328125" customWidth="1"/>
-    <col min="17" max="17" width="10" customWidth="1"/>
+    <col min="3" max="3" width="8.7265625" style="3"/>
+    <col min="4" max="4" width="11.54296875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="10" style="3" customWidth="1"/>
+    <col min="8" max="8" width="8.7265625" style="3"/>
+    <col min="9" max="9" width="9.6328125" style="3" customWidth="1"/>
+    <col min="12" max="12" width="8.7265625" style="3"/>
+    <col min="13" max="13" width="9.36328125" style="3" customWidth="1"/>
+    <col min="16" max="16" width="8.7265625" style="3"/>
+    <col min="17" max="17" width="10" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="29" x14ac:dyDescent="0.35">
-      <c r="A1" s="3"/>
-      <c r="B1" s="4"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="5" t="s">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="5" t="s">
+      <c r="E1" s="2"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="5" t="s">
+      <c r="I1" s="2"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="5" t="s">
+      <c r="M1" s="2"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="Q1" s="3"/>
+      <c r="Q1" s="2"/>
     </row>
     <row r="2" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4" t="s">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="1"/>
+      <c r="K2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6" t="s">
+      <c r="L2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="M2" s="6" t="s">
+      <c r="M2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N2" s="1"/>
+      <c r="O2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6" t="s">
+      <c r="P2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="P2" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q2" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="5">
+      <c r="Q2" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
         <v>2019</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="2">
         <v>58.39</v>
       </c>
       <c r="D3" s="2">
@@ -588,85 +591,85 @@
       <c r="E3" s="2">
         <v>58.39</v>
       </c>
-      <c r="F3" s="2"/>
+      <c r="F3" s="1"/>
       <c r="G3" s="1">
         <v>73</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3" s="2">
         <v>73.290000000000006</v>
       </c>
-      <c r="I3" s="1">
+      <c r="I3" s="2">
         <v>73.72</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1">
         <v>70.72</v>
       </c>
-      <c r="L3" s="1">
+      <c r="L3" s="2">
         <v>70.849999999999994</v>
       </c>
-      <c r="M3" s="1">
+      <c r="M3" s="2">
         <v>70.849999999999994</v>
       </c>
       <c r="N3" s="1"/>
       <c r="O3" s="1">
         <v>74.98</v>
       </c>
-      <c r="P3" s="1">
+      <c r="P3" s="2">
         <v>75.03</v>
       </c>
-      <c r="Q3" s="1">
+      <c r="Q3" s="2">
         <v>74.569999999999993</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="4"/>
-      <c r="B4" s="7" t="s">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="2">
         <v>67.349999999999994</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="2">
         <v>67.349999999999994</v>
       </c>
       <c r="E4" s="2">
         <v>67.349999999999994</v>
       </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2">
+      <c r="F4" s="1"/>
+      <c r="G4" s="1">
         <v>81.64</v>
       </c>
-      <c r="H4" s="1">
+      <c r="H4" s="2">
         <v>82.28</v>
       </c>
-      <c r="I4" s="1">
+      <c r="I4" s="2">
         <v>82.58</v>
       </c>
       <c r="J4" s="1"/>
       <c r="K4" s="1">
         <v>81.44</v>
       </c>
-      <c r="L4" s="1">
+      <c r="L4" s="2">
         <v>80.63</v>
       </c>
-      <c r="M4" s="1">
+      <c r="M4" s="2">
         <v>80.64</v>
       </c>
       <c r="N4" s="1"/>
       <c r="O4" s="1">
         <v>84.47</v>
       </c>
-      <c r="P4" s="1">
+      <c r="P4" s="2">
         <v>84.39</v>
       </c>
-      <c r="Q4" s="1">
+      <c r="Q4" s="2">
         <v>84.4</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="4"/>
-      <c r="B5" s="7" t="s">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="2">
@@ -678,346 +681,346 @@
       <c r="E5" s="2">
         <v>55.06</v>
       </c>
-      <c r="F5" s="2"/>
+      <c r="F5" s="1"/>
       <c r="G5" s="1">
         <v>72.680000000000007</v>
       </c>
-      <c r="H5" s="1">
+      <c r="H5" s="2">
         <v>71.790000000000006</v>
       </c>
-      <c r="I5" s="1">
+      <c r="I5" s="2">
         <v>73.14</v>
       </c>
       <c r="J5" s="1"/>
       <c r="K5" s="1">
         <v>58.99</v>
       </c>
-      <c r="L5" s="1">
-        <v>57.7</v>
-      </c>
-      <c r="M5" s="1">
+      <c r="L5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M5" s="2">
         <v>57.7</v>
       </c>
       <c r="N5" s="1"/>
       <c r="O5" s="1">
         <v>79.16</v>
       </c>
-      <c r="P5" s="1">
+      <c r="P5" s="2">
         <v>78.88</v>
       </c>
-      <c r="Q5" s="1">
+      <c r="Q5" s="2">
         <v>79.180000000000007</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="1"/>
-    </row>
-    <row r="7" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="5">
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
         <v>2020</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="2">
         <v>74.400000000000006</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="2">
         <v>74.400000000000006</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="2">
         <v>74.400000000000006</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1">
         <v>77.260000000000005</v>
       </c>
-      <c r="H7" s="1">
+      <c r="H7" s="2">
         <v>76.760000000000005</v>
       </c>
-      <c r="I7" s="1">
+      <c r="I7" s="2">
         <v>77.27</v>
       </c>
       <c r="J7" s="1"/>
       <c r="K7" s="1">
         <v>75.14</v>
       </c>
-      <c r="L7" s="1">
+      <c r="L7" s="2">
         <v>73.510000000000005</v>
       </c>
-      <c r="M7" s="1">
+      <c r="M7" s="2">
         <v>73.510000000000005</v>
       </c>
       <c r="N7" s="1"/>
       <c r="O7" s="1">
         <v>80.37</v>
       </c>
-      <c r="P7" s="1">
+      <c r="P7" s="2">
         <v>80.61</v>
       </c>
-      <c r="Q7" s="1">
+      <c r="Q7" s="2">
         <v>81.349999999999994</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="3"/>
-      <c r="B8" s="7" t="s">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="2">
         <v>67.599999999999994</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="2">
         <v>67.599999999999994</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="2">
         <v>67.599999999999994</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1">
         <v>82.46</v>
       </c>
-      <c r="H8" s="1">
+      <c r="H8" s="2">
         <v>82.14</v>
       </c>
-      <c r="I8" s="1">
+      <c r="I8" s="2">
         <v>82.89</v>
       </c>
       <c r="J8" s="1"/>
       <c r="K8" s="1">
         <v>76.42</v>
       </c>
-      <c r="L8" s="1">
+      <c r="L8" s="2">
         <v>75.319999999999993</v>
       </c>
-      <c r="M8" s="1">
+      <c r="M8" s="2">
         <v>75.319999999999993</v>
       </c>
       <c r="N8" s="1"/>
       <c r="O8" s="1">
         <v>84.95</v>
       </c>
-      <c r="P8" s="1">
+      <c r="P8" s="2">
         <v>85.01</v>
       </c>
-      <c r="Q8" s="1">
+      <c r="Q8" s="2">
         <v>84.81</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="3"/>
-      <c r="B9" s="7" t="s">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="2">
         <v>58.63</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="2">
         <v>58.63</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="2">
         <v>58.63</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1">
         <v>75.42</v>
       </c>
-      <c r="H9" s="1">
+      <c r="H9" s="2">
         <v>77.55</v>
       </c>
-      <c r="I9" s="1">
+      <c r="I9" s="2">
         <v>78.33</v>
       </c>
       <c r="J9" s="1"/>
       <c r="K9" s="1">
         <v>74.97</v>
       </c>
-      <c r="L9" s="1">
+      <c r="L9" s="2">
         <v>76</v>
       </c>
-      <c r="M9" s="1">
+      <c r="M9" s="2">
         <v>76</v>
       </c>
       <c r="N9" s="1"/>
       <c r="O9" s="1">
         <v>82.46</v>
       </c>
-      <c r="P9" s="1">
+      <c r="P9" s="2">
         <v>82.21</v>
       </c>
-      <c r="Q9" s="1">
+      <c r="Q9" s="2">
         <v>82.75</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="1"/>
-    </row>
-    <row r="11" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="7" t="s">
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="2">
         <v>65.95</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="2">
         <v>65.95</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="2">
         <v>58.39</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1">
         <v>76.09</v>
       </c>
-      <c r="H11" s="1">
+      <c r="H11" s="2">
         <v>75.989999999999995</v>
       </c>
-      <c r="I11" s="1">
+      <c r="I11" s="2">
         <v>73.72</v>
       </c>
       <c r="J11" s="1"/>
       <c r="K11" s="1">
         <v>73.73</v>
       </c>
-      <c r="L11" s="1">
+      <c r="L11" s="2">
         <v>73.52</v>
       </c>
-      <c r="M11" s="1">
+      <c r="M11" s="2">
         <v>70.849999999999994</v>
       </c>
       <c r="N11" s="1"/>
       <c r="O11" s="1">
         <v>77.88</v>
       </c>
-      <c r="P11" s="1">
+      <c r="P11" s="2">
         <v>77.88</v>
       </c>
-      <c r="Q11" s="1">
+      <c r="Q11" s="2">
         <v>74.569999999999993</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="3"/>
-      <c r="B12" s="7" t="s">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="2">
         <v>62.58</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="2">
         <v>62.58</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12" s="2">
         <v>62.58</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1">
         <v>78.790000000000006</v>
       </c>
-      <c r="H12" s="1">
+      <c r="H12" s="2">
         <v>79.17</v>
       </c>
-      <c r="I12" s="1">
+      <c r="I12" s="2">
         <v>80.099999999999994</v>
       </c>
       <c r="J12" s="1"/>
       <c r="K12" s="1">
         <v>79.89</v>
       </c>
-      <c r="L12" s="1">
+      <c r="L12" s="2">
         <v>79.67</v>
       </c>
-      <c r="M12" s="1">
+      <c r="M12" s="2">
         <v>79.67</v>
       </c>
       <c r="N12" s="1"/>
       <c r="O12" s="1">
         <v>81.010000000000005</v>
       </c>
-      <c r="P12" s="1">
+      <c r="P12" s="2">
         <v>80.94</v>
       </c>
-      <c r="Q12" s="1">
+      <c r="Q12" s="2">
         <v>80.86</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="3"/>
-      <c r="B13" s="7" t="s">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="2">
         <v>47.83</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13" s="2">
         <v>47.83</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13" s="2">
         <v>47.83</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1">
         <v>70.36</v>
       </c>
-      <c r="H13" s="1">
+      <c r="H13" s="2">
         <v>71.86</v>
       </c>
-      <c r="I13" s="1">
+      <c r="I13" s="2">
         <v>72.88</v>
       </c>
       <c r="J13" s="1"/>
       <c r="K13" s="1">
         <v>65.849999999999994</v>
       </c>
-      <c r="L13" s="1">
+      <c r="L13" s="2">
         <v>65.849999999999994</v>
       </c>
-      <c r="M13" s="1">
+      <c r="M13" s="2">
         <v>65.849999999999994</v>
       </c>
       <c r="N13" s="1"/>
       <c r="O13" s="1">
         <v>77.77</v>
       </c>
-      <c r="P13" s="1">
+      <c r="P13" s="2">
         <v>77.680000000000007</v>
       </c>
-      <c r="Q13" s="1">
+      <c r="Q13" s="2">
         <v>77.67</v>
       </c>
     </row>
@@ -1025,4 +1028,73 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34C391F0-6045-4D3B-B47C-4C0D42D90B5C}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1.444758</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1.6603019999999999</v>
+      </c>
+      <c r="D2" s="1">
+        <v>2.4212359999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2.080104</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1.675897</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1.7453529999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1.242442</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.58439399999999997</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.51166880000000003</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>